<commit_message>
OFF Days for different batches done
</commit_message>
<xml_diff>
--- a/20_routineData.xlsx
+++ b/20_routineData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anika Tabassum\Desktop\blinkproject_new\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB84419-0BCD-4E7A-AFB3-E36B009ECFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032713C2-6598-45DD-A045-56C98972BFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="31">
   <si>
     <t>batch</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>14:00</t>
+  </si>
+  <si>
+    <t>brintaa</t>
   </si>
 </sst>
 </file>
@@ -492,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -532,7 +535,7 @@
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -946,7 +949,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 A3:E5 A2:B2 E2 A7:E25 A6:B6 A26:B26" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E1 A3:E5 A2:B2 A7:E25 A6:B6 A26:B26" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>